<commit_message>
Planejamento do primeiro semestre
</commit_message>
<xml_diff>
--- a/planejamento/cronograma.xlsx
+++ b/planejamento/cronograma.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="CAPACIDADES" sheetId="1" r:id="rId1"/>
@@ -21776,8 +21776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CV1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BA1" workbookViewId="0">
-      <selection sqref="A1:CV1"/>
+    <sheetView topLeftCell="BA1" workbookViewId="0">
+      <selection activeCell="BN8" sqref="BN8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24314,9 +24314,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CX71"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AV1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A71" sqref="A71"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25003,7 +25003,9 @@
       <c r="B7" s="88"/>
       <c r="C7" s="65"/>
       <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
+      <c r="E7" s="65">
+        <v>2</v>
+      </c>
       <c r="P7" s="228"/>
       <c r="Q7" s="87"/>
       <c r="R7" s="88"/>

</xml_diff>